<commit_message>
Excellent progress tonight on issue reporting, image and link checking.
</commit_message>
<xml_diff>
--- a/Project/Reports/Services Australia - Diploma - BP - 202X Cohort X MIP_CanvasValidationReport.xlsx
+++ b/Project/Reports/Services Australia - Diploma - BP - 202X Cohort X MIP_CanvasValidationReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Wisdom canvas error report</t>
   </si>
@@ -37,16 +37,22 @@
     <t>Participants</t>
   </si>
   <si>
-    <t>Pages</t>
-  </si>
-  <si>
-    <t>Modules</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Page count</t>
+  </si>
+  <si>
+    <t>Module count</t>
+  </si>
+  <si>
+    <t>Assessment count</t>
   </si>
   <si>
     <t>Time taken to generate</t>
   </si>
   <si>
-    <t>16.98</t>
+    <t>74.2</t>
   </si>
 </sst>
 </file>
@@ -391,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -434,32 +440,45 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
+      <c r="B5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>10</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B6" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>